<commit_message>
modified:   m_apex_adjust_01.xlsx 	modified:   m_apex_adjust_02.xlsx 	modified:   m_apex_adjust_03.xlsx
</commit_message>
<xml_diff>
--- a/m_apex_adjust_01.xlsx
+++ b/m_apex_adjust_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUF\00_TitanTwo\01_devProject\01_M_ApexLegends\01_cv_premium_apexcv_yyds_s17\dev_scripts\GCV\v9_m\916m_v120m_dev_20240701\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE221D3F-8DA3-4C3E-BA69-2FEA0A848335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F9F8FE-7895-4152-9E3C-ECC8C6E9A3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19425" yWindow="1995" windowWidth="19395" windowHeight="20250" tabRatio="812" firstSheet="16" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5850" yWindow="5850" windowWidth="43185" windowHeight="23445" tabRatio="812" firstSheet="16" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NONE" sheetId="6" r:id="rId1"/>
@@ -7007,7 +7007,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7058,7 +7058,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="13">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>

</xml_diff>